<commit_message>
some work is done on the test file and a utils file is created
</commit_message>
<xml_diff>
--- a/Plan+tests+acceptation_P5_TB.xlsx
+++ b/Plan+tests+acceptation_P5_TB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t xml:space="preserve">Fonctionnalité</t>
   </si>
@@ -49,46 +49,55 @@
     <t xml:space="preserve">allProductsFromAPI() (dans script.js)</t>
   </si>
   <si>
+    <t xml:space="preserve">action pour déclencher la fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On requête l'API pour récupérer tous les produits et les afficher correctement dans la page d'index</t>
+  </si>
+  <si>
     <t xml:space="preserve">oneProductFromAPI() (dans product.js)</t>
   </si>
   <si>
     <t xml:space="preserve">numStr(a, b) (dans product.js et cart.js)</t>
   </si>
   <si>
+    <t xml:space="preserve">On passe le nombre « a » en paramètre pour obtenir le même nombre mais en chaîne de caractère et avec un séparateur de millier (le paramètre « b » qui est par défaut un espace)</t>
+  </si>
+  <si>
     <t xml:space="preserve">getProductsData() (dans cart.js)</t>
   </si>
   <si>
+    <t xml:space="preserve">On créé une fonction pour récupérer les bonnes données (dans le localStorage et en requêtant l’API), et les afficher dynamiquement sur la page cart. La gestion de modification / suppression de quantité dans le panier est également géré dans cette fonction.</t>
+  </si>
+  <si>
     <t xml:space="preserve">getDatasFromId(id) (dans cart.js)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">getTotalQuantity() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">(dans cart.js)</t>
-    </r>
+    <t xml:space="preserve">fonction qui prend en paramètre l'id du produit et qui renvoie les données correspondantes dont nous aurons besoin (hors ce qui est déja stocké dans le localStorage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getTotalQuantity() (dans cart.js)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction permettant d'afficher la quantité totale de products dans le panier </t>
   </si>
   <si>
     <t xml:space="preserve">getTotalCartPrice() (dans cart.js)</t>
   </si>
   <si>
+    <t xml:space="preserve">fonction permettant de récupèrer le montant total du panier</t>
+  </si>
+  <si>
     <t xml:space="preserve">checkFormAndPostRequest() (dans cart.js)</t>
   </si>
   <si>
+    <t xml:space="preserve">fonction qui va vérifier la validité du formulaire et envoyer la requête POST à l'API si valide (au clic du bouton "Commander !")</t>
+  </si>
+  <si>
     <t xml:space="preserve">displayOrderId() (dans confirmation.js)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On récupère l'orderId dans l'url de la page courrante puis on se place au bon endroit de la page et on y affiche l'orderId </t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -142,21 +151,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Montserrat"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,7 +162,37 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEC9BA4"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF819E"/>
+        <bgColor rgb="FFEC9BA4"/>
       </patternFill>
     </fill>
   </fills>
@@ -316,7 +342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,19 +383,71 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,7 +496,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -439,9 +517,9 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFE8F2A1"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFEC9BA4"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -451,7 +529,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -473,14 +551,14 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.71"/>
   </cols>
   <sheetData>
@@ -516,16 +594,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -533,181 +615,195 @@
       <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8" t="s">
+      <c r="B11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="14"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="14"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="14"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
the test file is now completed
</commit_message>
<xml_diff>
--- a/Plan+tests+acceptation_P5_TB.xlsx
+++ b/Plan+tests+acceptation_P5_TB.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille 1_2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille 1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t xml:space="preserve">Fonctionnalité</t>
   </si>
@@ -44,6 +45,130 @@
   </si>
   <si>
     <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choix d’un des produits depuis la page d’accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clic du produit choisi par l’utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction de l’utilisateur vers la page du produit sélectionné</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Une page « produit » où on affiche une image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> du produit sélectionné avec toutes ses informations</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’image du produit sélectionnée est la bonne et toutes les informations relatives au produit sont correctement affichées.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choix d’une couleur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> et d’une quantité sur la page du produit</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Clic sur le sélecteur de couleur et sur le sélecteur de quantité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au clic du sélecteur de couleur, toutes les couleurs possibles pour le produit sélectionné s’affichent. Au clic d’une couleur, la couleur sélectionnée reste affichée. La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des produits au panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clic sur le bouton « Ajouter au Panier »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Après le clic, le local storage du navigateur récupère l’id du produit sélectionné, la couleur choisie et la quantité retenue. Si un article similaire (id et couleur) est déjà présent dans le local storage, la nouvelle quantité s’ajoute à celle déjà présente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une page « panier » affichant tous les articles que l’utilisateur a ajouté dans son panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clic dans la partie navigation du site sur « Panier »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de l'ensemble des produits du panier de l’utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustement dynamique des quantités du panier depuis la page panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clic sur le sélecteur de quantité et sur le bouton « Supprimer » pour chaque produit du panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -). Le produit disparaît de la page dès que l’utilisateur clic sur le bouton « Supprimer »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage dynamique du nombre total d’articles dans le panier et du montant total du panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’affichage est automatiquement mis à jour en fonction de l’ajustement des quantités par l’utilisateur sur la page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage d’une alerte au chargement de la page panier si le panier est vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A l’arrivée sur la page panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une alerte est affichée permettant à l’utilisateur de comprendre qu’il doit d’abord ajouter des articles dans son panier avant de venir sur cette page pour y faire quelques-chose.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renseignement des coordonnées du client avant sa commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renseignement des champs du formulaire puis clic sur le bouton « Commander ! ». </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour permettre la commande, tous les champs du formulaire doivent être remplis et l’adresse email doit avoir une forme valide (sinon, ajout dynamique de message d’erreurs adaptés) et le panier doit contenir au moins 1 article au moment du clic. Si ces conditions sont remplies, on dirige l’utilisateur vers la page de confirmation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une page « confirmation » qui affiche le numéro de commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage du numéro de commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur cette page, on indique dans un message à l’utilisateur son numéro de commande.</t>
   </si>
   <si>
     <t xml:space="preserve">allProductsFromAPI() (dans script.js)</t>
@@ -107,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -150,6 +275,17 @@
       <name val="Montserrat"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Montserrat"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Montserrat"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -342,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,63 +519,27 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,6 +569,66 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -548,13 +708,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.41"/>
@@ -594,20 +754,326 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="99.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="B3" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -615,12 +1081,12 @@
       <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15" t="s">
+      <c r="B4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28" t="s">
         <v>7</v>
       </c>
     </row>
@@ -628,14 +1094,14 @@
       <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="B5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>7</v>
       </c>
     </row>
@@ -643,14 +1109,14 @@
       <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="21" t="s">
+      <c r="B6" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -658,14 +1124,14 @@
       <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="21" t="s">
+      <c r="B7" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -673,14 +1139,14 @@
       <c r="A8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="B8" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -688,14 +1154,14 @@
       <c r="A9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="21" t="s">
+      <c r="B9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -703,14 +1169,14 @@
       <c r="A10" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="21" t="s">
+      <c r="B10" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -718,92 +1184,92 @@
       <c r="A11" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="B11" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
the utils script is now called on 2 pages + 2 unusefull functions have been deleted on cart page
</commit_message>
<xml_diff>
--- a/Plan+tests+acceptation_P5_TB.xlsx
+++ b/Plan+tests+acceptation_P5_TB.xlsx
@@ -38,137 +38,453 @@
     <t xml:space="preserve">Une page d’accueil montrant (de manière dynamique) tous les articles disponibles à la vente.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ouvrir sur la page d'accueil du site web dans un navigateur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de l'ensemble des produits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choix d’un des produits depuis la page d’accueil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clic du produit choisi par l’utilisateur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction de l’utilisateur vers la page du produit sélectionné.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Une page « produit » où on affiche une image du produit sélectionné avec toutes ses informations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">L’image du produit sélectionnée est la bonne et toutes les informations relatives au produit sont correctement affichées</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choix d’une couleur et d’une quantité sur la page du produit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clic sur le sélecteur de couleur et sur le sélecteur de quantité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Au clic du sélecteur de couleur, toutes les couleurs possibles pour le produit sélectionné s’affichent. Au clic d’une couleur, la couleur sélectionnée reste affichée. La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ajout des produits au panier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clic sur le bouton « Ajouter au Panier »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Après le clic, le local storage du navigateur récupère l’id du produit sélectionné, la couleur choisie et la quantité retenue. Si un article similaire (id et couleur) est déjà présent dans le local storage, la nouvelle quantité s’ajoute à celle déjà présente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Une page « panier » affichant tous les articles que l’utilisateur a ajouté dans son panier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clic dans la partie navigation du site sur « Panier »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Affichage de l'ensemble des produits du panier de l’utilisateur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ajustement dynamique des quantités du panier depuis la page panier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clic sur le sélecteur de quantité et sur le bouton « Supprimer » pour chaque produit du panier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -). Le produit disparaît de la page dès que l’utilisateur clic sur le bouton « Supprimer »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Affichage dynamique du nombre total d’articles dans le panier et du montant total du panier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">L’affichage est automatiquement mis à jour en fonction de l’ajustement des quantités par l’utilisateur sur la page.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Affichage d’une alerte au chargement de la page panier si le panier est vide</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Une alerte est affichée permettant à l’utilisateur de comprendre qu’il doit d’abord ajouter des articles dans son panier avant de venir sur cette page pour y faire quelques-chose.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Renseignement des coordonnées du client avant sa commande</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Renseignement des champs du formulaire puis clic sur le bouton « Commander ! »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour permettre la commande, tous les champs du formulaire doivent être remplis et l’adresse email doit avoir une forme valide (sinon, ajout dynamique de message d’erreurs adaptés) et le panier doit contenir au moins 1 article au moment du clic. Si ces conditions sont remplies, on dirige l’utilisateur vers la page de confirmation.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Une page « confirmation » qui affiche le numéro de commande</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur cette page, on indique dans un message à l’utilisateur son numéro de commande. Le panier qui a été confirmé est automatiquement vidé.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ouvrir sur la page d'accueil du site web dans un navigateur</t>
   </si>
   <si>
     <t xml:space="preserve">Affichage de l'ensemble des produits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choix d’un des produits depuis la page d’accueil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clic du produit choisi par l’utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction de l’utilisateur vers la page du produit sélectionné</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Une page « produit » où on affiche une image</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> du produit sélectionné avec toutes ses informations</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’image du produit sélectionnée est la bonne et toutes les informations relatives au produit sont correctement affichées.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choix d’une couleur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> et d’une quantité sur la page du produit</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Clic sur le sélecteur de couleur et sur le sélecteur de quantité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Au clic du sélecteur de couleur, toutes les couleurs possibles pour le produit sélectionné s’affichent. Au clic d’une couleur, la couleur sélectionnée reste affichée. La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajout des produits au panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clic sur le bouton « Ajouter au Panier »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Après le clic, le local storage du navigateur récupère l’id du produit sélectionné, la couleur choisie et la quantité retenue. Si un article similaire (id et couleur) est déjà présent dans le local storage, la nouvelle quantité s’ajoute à celle déjà présente.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une page « panier » affichant tous les articles que l’utilisateur a ajouté dans son panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clic dans la partie navigation du site sur « Panier »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage de l'ensemble des produits du panier de l’utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajustement dynamique des quantités du panier depuis la page panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clic sur le sélecteur de quantité et sur le bouton « Supprimer » pour chaque produit du panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La quantité affichée réagit immédiatement en fonction des clics sur le sélecteur de quantité (en + comme en -). Le produit disparaît de la page dès que l’utilisateur clic sur le bouton « Supprimer »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage dynamique du nombre total d’articles dans le panier et du montant total du panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’affichage est automatiquement mis à jour en fonction de l’ajustement des quantités par l’utilisateur sur la page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage d’une alerte au chargement de la page panier si le panier est vide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A l’arrivée sur la page panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une alerte est affichée permettant à l’utilisateur de comprendre qu’il doit d’abord ajouter des articles dans son panier avant de venir sur cette page pour y faire quelques-chose.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renseignement des coordonnées du client avant sa commande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renseignement des champs du formulaire puis clic sur le bouton « Commander ! ». </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour permettre la commande, tous les champs du formulaire doivent être remplis et l’adresse email doit avoir une forme valide (sinon, ajout dynamique de message d’erreurs adaptés) et le panier doit contenir au moins 1 article au moment du clic. Si ces conditions sont remplies, on dirige l’utilisateur vers la page de confirmation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une page « confirmation » qui affiche le numéro de commande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage du numéro de commande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sur cette page, on indique dans un message à l’utilisateur son numéro de commande.</t>
   </si>
   <si>
     <t xml:space="preserve">allProductsFromAPI() (dans script.js)</t>
@@ -278,12 +594,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Montserrat"/>
       <family val="0"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF000000"/>
       <name val="Montserrat"/>
       <family val="0"/>
     </font>
@@ -478,7 +794,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,31 +839,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,11 +1006,11 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.41"/>
@@ -754,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
@@ -799,11 +1095,11 @@
       <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="99.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="100.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
         <v>4</v>
       </c>
@@ -844,10 +1140,10 @@
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -864,7 +1160,7 @@
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -879,10 +1175,10 @@
         <v>29</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>7</v>
@@ -893,110 +1189,110 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1020,7 +1316,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.41"/>
@@ -1051,10 +1347,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>7</v>
@@ -1064,16 +1360,16 @@
       <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1081,12 +1377,12 @@
       <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1094,14 +1390,14 @@
       <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1109,14 +1405,14 @@
       <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1124,14 +1420,14 @@
       <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1139,14 +1435,14 @@
       <c r="A8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1154,14 +1450,14 @@
       <c r="A9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1169,14 +1465,14 @@
       <c r="A10" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1184,92 +1480,92 @@
       <c r="A11" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>